<commit_message>
adding the basic functionality to categorize transactions based on predefined categories.
</commit_message>
<xml_diff>
--- a/עובר ושב_09092025_1744.xlsx
+++ b/עובר ושב_09092025_1744.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7f4f491ad4f85a7/Documents/GitHub/Consolidation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_C3466D6CF965FF08F87BB67AD726DABA0F04D8FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_C3466D6CF965FF08F87BB67AD726DABA0F04D8FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86EDEE08-F1E3-4E58-A715-DA5C8EB79AF9}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="עובר ושב" sheetId="1" r:id="rId1"/>
@@ -726,14 +726,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="7" width="9.7109375" customWidth="1"/>
@@ -741,42 +741,42 @@
     <col min="9" max="9" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -802,7 +802,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>45907</v>
       </c>
@@ -828,7 +828,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>45907</v>
       </c>
@@ -854,7 +854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>45904</v>
       </c>
@@ -880,7 +880,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>45902</v>
       </c>
@@ -906,7 +906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>45902</v>
       </c>
@@ -932,7 +932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>45901</v>
       </c>
@@ -958,7 +958,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>45898</v>
       </c>
@@ -984,7 +984,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>45888</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>45888</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>45887</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>45884</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>45883</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>45882</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>45879</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>45879</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>45879</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>45879</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>45879</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>45876</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>45876</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>45875</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>45873</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>45873</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>45873</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>45868</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>45865</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>45861</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>45860</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>45856</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>45855</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>45848</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>45848</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>45848</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>45848</v>
       </c>
@@ -1686,17 +1686,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>5</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>45881</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>45881</v>
       </c>

</xml_diff>